<commit_message>
RESTful API für Benutzer anlegen, updaten, löschen, auswählen ist fertig
</commit_message>
<xml_diff>
--- a/REST_API/REST_API.xlsx
+++ b/REST_API/REST_API.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Methode</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Lösche den Benutzer mit der ID [{id}]</t>
+  </si>
+  <si>
+    <t>Grad</t>
+  </si>
+  <si>
+    <t>fertig</t>
   </si>
 </sst>
 </file>
@@ -113,12 +119,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:D5" totalsRowShown="0">
+  <autoFilter ref="A1:D5"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Methode"/>
     <tableColumn id="2" name="URL"/>
     <tableColumn id="3" name="Aktion"/>
+    <tableColumn id="4" name="Grad"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -387,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,7 +407,7 @@
     <col min="3" max="3" width="114.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,8 +417,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -421,8 +431,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -432,8 +445,11 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -443,8 +459,11 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -453,6 +472,9 @@
       </c>
       <c r="C5" t="s">
         <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel ergänzt und beispiel .json für den Login hinzugefügt
</commit_message>
<xml_diff>
--- a/REST_API/REST_API.xlsx
+++ b/REST_API/REST_API.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="42">
   <si>
     <t>Methode</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>getestet</t>
+  </si>
+  <si>
+    <t>/user/login</t>
+  </si>
+  <si>
+    <t>Loginfunktion, welche das Passwortwort überprüft</t>
   </si>
 </sst>
 </file>
@@ -194,8 +200,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:E18" totalsRowShown="0">
-  <autoFilter ref="A1:E18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:E19" totalsRowShown="0">
+  <autoFilter ref="A1:E19"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Methode"/>
     <tableColumn id="2" name="URL"/>
@@ -470,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,10 +511,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -519,13 +525,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -536,13 +542,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -553,13 +559,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -573,10 +579,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -590,10 +596,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -607,10 +613,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -624,10 +630,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -641,10 +647,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -655,13 +661,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -672,13 +678,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -689,13 +695,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -709,10 +715,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -723,13 +729,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
@@ -740,13 +746,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
@@ -760,10 +766,10 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
@@ -774,18 +780,35 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
       </c>
       <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
         <v>32</v>
       </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>